<commit_message>
CIDC-1303 first pass at classifying ids
</commit_message>
<xml_diff>
--- a/template_examples/wes_fastq_template.xlsx
+++ b/template_examples/wes_fastq_template.xlsx
@@ -216,7 +216,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2124" uniqueCount="81">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2133" uniqueCount="90">
   <si>
     <t xml:space="preserve">#title</t>
   </si>
@@ -330,6 +330,33 @@
   </si>
   <si>
     <t xml:space="preserve">/local/path/to/rev.1.2.1_2.fastq.gz</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CTTTPP122.00</t>
+  </si>
+  <si>
+    <t xml:space="preserve">/local/path/to/fwd.1.2.2.fastq.gz</t>
+  </si>
+  <si>
+    <t xml:space="preserve">/local/path/to/rev.1.2.2.fastq.gz</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CTTTPP123.00</t>
+  </si>
+  <si>
+    <t xml:space="preserve">/local/path/to/fwd.1.2.3.fastq.gz</t>
+  </si>
+  <si>
+    <t xml:space="preserve">/local/path/to/rev.1.2.3.fastq.gz</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CTTTPP124.00</t>
+  </si>
+  <si>
+    <t xml:space="preserve">/local/path/to/fwd.1.2.4.fastq.gz</t>
+  </si>
+  <si>
+    <t xml:space="preserve">/local/path/to/rev.1.2.4.fastq.gz</t>
   </si>
   <si>
     <t xml:space="preserve">LEGEND</t>
@@ -469,7 +496,7 @@
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="m/d/yyyy"/>
   </numFmts>
-  <fonts count="7">
+  <fonts count="6">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -499,12 +526,6 @@
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="1"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF000000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
     </font>
     <font>
       <sz val="10"/>
@@ -619,7 +640,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -706,11 +727,11 @@
   </sheetPr>
   <dimension ref="A1:G2012"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E4" activeCellId="0" sqref="E4"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B20" activeCellId="0" sqref="B20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.28125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.30078125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="101" min="1" style="0" width="30.7"/>
   </cols>
@@ -940,19 +961,73 @@
         <v>1</v>
       </c>
     </row>
-    <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="0" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B17" s="0" t="s">
+        <v>38</v>
+      </c>
+      <c r="C17" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="D17" s="0" t="s">
+        <v>39</v>
+      </c>
+      <c r="E17" s="0" t="s">
+        <v>40</v>
+      </c>
+      <c r="F17" s="4" t="n">
+        <v>40179</v>
+      </c>
+      <c r="G17" s="0" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="0" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B18" s="0" t="s">
+        <v>41</v>
+      </c>
+      <c r="C18" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="D18" s="0" t="s">
+        <v>42</v>
+      </c>
+      <c r="E18" s="0" t="s">
+        <v>43</v>
+      </c>
+      <c r="F18" s="4" t="n">
+        <v>40179</v>
+      </c>
+      <c r="G18" s="0" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="0" t="s">
         <v>27</v>
+      </c>
+      <c r="B19" s="0" t="s">
+        <v>44</v>
+      </c>
+      <c r="C19" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="D19" s="0" t="s">
+        <v>45</v>
+      </c>
+      <c r="E19" s="0" t="s">
+        <v>46</v>
+      </c>
+      <c r="F19" s="4" t="n">
+        <v>40179</v>
+      </c>
+      <c r="G19" s="0" t="n">
+        <v>1</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -10926,7 +11001,7 @@
     <mergeCell ref="B11:G11"/>
   </mergeCells>
   <dataValidations count="6">
-    <dataValidation allowBlank="true" error="Please enter date in format mm/dd/yyyy" errorStyle="stop" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="F17:F2012" type="custom">
+    <dataValidation allowBlank="true" error="Please enter date in format mm/dd/yyyy" errorStyle="stop" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="F20:F2012" type="custom">
       <formula1>AND(ISNUMBER(F13:F2012),LEFT(CELL("format",F13:F2012),1)="D")</formula1>
       <formula2>0</formula2>
     </dataValidation>
@@ -10973,19 +11048,19 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.28125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.30078125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="101" min="2" style="0" width="30.7"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B1" s="6" t="s">
-        <v>38</v>
+        <v>47</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B2" s="1" t="s">
-        <v>39</v>
+        <v>48</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -10993,10 +11068,10 @@
         <v>3</v>
       </c>
       <c r="C3" s="0" t="s">
-        <v>40</v>
+        <v>49</v>
       </c>
       <c r="D3" s="0" t="s">
-        <v>41</v>
+        <v>50</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -11004,13 +11079,13 @@
         <v>5</v>
       </c>
       <c r="C4" s="0" t="s">
-        <v>42</v>
+        <v>51</v>
       </c>
       <c r="D4" s="0" t="s">
-        <v>43</v>
+        <v>52</v>
       </c>
       <c r="E4" s="0" t="s">
-        <v>44</v>
+        <v>53</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -11018,13 +11093,13 @@
         <v>7</v>
       </c>
       <c r="C5" s="0" t="s">
-        <v>42</v>
+        <v>51</v>
       </c>
       <c r="D5" s="0" t="s">
-        <v>45</v>
+        <v>54</v>
       </c>
       <c r="E5" s="0" t="s">
-        <v>46</v>
+        <v>55</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -11032,13 +11107,13 @@
         <v>9</v>
       </c>
       <c r="C6" s="0" t="s">
-        <v>42</v>
+        <v>51</v>
       </c>
       <c r="D6" s="0" t="s">
-        <v>47</v>
+        <v>56</v>
       </c>
       <c r="E6" s="0" t="s">
-        <v>48</v>
+        <v>57</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -11046,13 +11121,13 @@
         <v>11</v>
       </c>
       <c r="C7" s="0" t="s">
-        <v>42</v>
+        <v>51</v>
       </c>
       <c r="D7" s="0" t="s">
-        <v>49</v>
+        <v>58</v>
       </c>
       <c r="E7" s="0" t="s">
-        <v>50</v>
+        <v>59</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -11060,13 +11135,13 @@
         <v>13</v>
       </c>
       <c r="C8" s="0" t="s">
-        <v>42</v>
+        <v>51</v>
       </c>
       <c r="D8" s="0" t="s">
-        <v>51</v>
+        <v>60</v>
       </c>
       <c r="E8" s="0" t="s">
-        <v>52</v>
+        <v>61</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -11074,10 +11149,10 @@
         <v>15</v>
       </c>
       <c r="C9" s="0" t="s">
-        <v>53</v>
+        <v>62</v>
       </c>
       <c r="D9" s="0" t="s">
-        <v>54</v>
+        <v>63</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -11085,18 +11160,18 @@
         <v>16</v>
       </c>
       <c r="C10" s="0" t="s">
-        <v>42</v>
+        <v>51</v>
       </c>
       <c r="D10" s="0" t="s">
-        <v>55</v>
+        <v>64</v>
       </c>
       <c r="E10" s="0" t="s">
-        <v>56</v>
+        <v>65</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B11" s="1" t="s">
-        <v>57</v>
+        <v>66</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -11104,13 +11179,13 @@
         <v>21</v>
       </c>
       <c r="C12" s="0" t="s">
-        <v>58</v>
+        <v>67</v>
       </c>
       <c r="D12" s="0" t="s">
-        <v>59</v>
+        <v>68</v>
       </c>
       <c r="E12" s="0" t="s">
-        <v>60</v>
+        <v>69</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -11118,7 +11193,7 @@
         <v>22</v>
       </c>
       <c r="C13" s="0" t="s">
-        <v>40</v>
+        <v>49</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -11126,10 +11201,10 @@
         <v>23</v>
       </c>
       <c r="C14" s="0" t="s">
-        <v>40</v>
+        <v>49</v>
       </c>
       <c r="D14" s="0" t="s">
-        <v>61</v>
+        <v>70</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -11137,10 +11212,10 @@
         <v>24</v>
       </c>
       <c r="C15" s="0" t="s">
-        <v>40</v>
+        <v>49</v>
       </c>
       <c r="D15" s="0" t="s">
-        <v>61</v>
+        <v>70</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -11148,10 +11223,10 @@
         <v>25</v>
       </c>
       <c r="C16" s="0" t="s">
-        <v>62</v>
+        <v>71</v>
       </c>
       <c r="D16" s="0" t="s">
-        <v>63</v>
+        <v>72</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -11159,10 +11234,10 @@
         <v>26</v>
       </c>
       <c r="C17" s="0" t="s">
-        <v>64</v>
+        <v>73</v>
       </c>
       <c r="D17" s="0" t="s">
-        <v>65</v>
+        <v>74</v>
       </c>
     </row>
   </sheetData>
@@ -11188,7 +11263,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.28125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.30078125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="101" min="2" style="0" width="30.7"/>
   </cols>
@@ -11215,7 +11290,7 @@
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B2" s="0" t="s">
-        <v>66</v>
+        <v>75</v>
       </c>
       <c r="C2" s="0" t="s">
         <v>8</v>
@@ -11224,7 +11299,7 @@
         <v>10</v>
       </c>
       <c r="E2" s="0" t="s">
-        <v>67</v>
+        <v>76</v>
       </c>
       <c r="F2" s="0" t="s">
         <v>14</v>
@@ -11238,54 +11313,54 @@
         <v>6</v>
       </c>
       <c r="C3" s="0" t="s">
-        <v>68</v>
+        <v>77</v>
       </c>
       <c r="D3" s="0" t="s">
-        <v>69</v>
+        <v>78</v>
       </c>
       <c r="E3" s="0" t="s">
-        <v>70</v>
+        <v>79</v>
       </c>
       <c r="F3" s="0" t="s">
-        <v>71</v>
+        <v>80</v>
       </c>
       <c r="G3" s="0" t="s">
-        <v>72</v>
+        <v>81</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B4" s="0" t="s">
-        <v>73</v>
+        <v>82</v>
       </c>
       <c r="D4" s="0" t="s">
-        <v>74</v>
+        <v>83</v>
       </c>
       <c r="E4" s="0" t="s">
         <v>12</v>
       </c>
       <c r="G4" s="0" t="s">
-        <v>75</v>
+        <v>84</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B5" s="0" t="s">
-        <v>76</v>
+        <v>85</v>
       </c>
       <c r="D5" s="0" t="s">
-        <v>77</v>
+        <v>86</v>
       </c>
       <c r="E5" s="0" t="s">
-        <v>78</v>
+        <v>87</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E6" s="0" t="s">
-        <v>79</v>
+        <v>88</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E7" s="0" t="s">
-        <v>80</v>
+        <v>89</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
CIDC-1508 use bam and fastq for pairing test
</commit_message>
<xml_diff>
--- a/template_examples/wes_fastq_template.xlsx
+++ b/template_examples/wes_fastq_template.xlsx
@@ -216,7 +216,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2185" uniqueCount="141">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2179" uniqueCount="135">
   <si>
     <t xml:space="preserve">#title</t>
   </si>
@@ -302,36 +302,6 @@
     <t xml:space="preserve">#data</t>
   </si>
   <si>
-    <t xml:space="preserve">CTTTPP111.00</t>
-  </si>
-  <si>
-    <t xml:space="preserve">/local/path/to/fwd.1.1.1.fastq.gz</t>
-  </si>
-  <si>
-    <t xml:space="preserve">/local/path/to/rev.1.1.1.fastq.gz</t>
-  </si>
-  <si>
-    <t xml:space="preserve">CTTTPP121.00</t>
-  </si>
-  <si>
-    <t xml:space="preserve">/local/path/to/fwd.1.2.1.fastq.gz</t>
-  </si>
-  <si>
-    <t xml:space="preserve">/local/path/to/rev.1.2.1.fastq.gz</t>
-  </si>
-  <si>
-    <t xml:space="preserve">/local/path/to/fwd.1.1.1_2.fastq.gz</t>
-  </si>
-  <si>
-    <t xml:space="preserve">/local/path/to/rev.1.1.1_2.fastq.gz</t>
-  </si>
-  <si>
-    <t xml:space="preserve">/local/path/to/fwd.1.2.1_2.fastq.gz</t>
-  </si>
-  <si>
-    <t xml:space="preserve">/local/path/to/rev.1.2.1_2.fastq.gz</t>
-  </si>
-  <si>
     <t xml:space="preserve">CTTTPP122.00</t>
   </si>
   <si>
@@ -348,6 +318,18 @@
   </si>
   <si>
     <t xml:space="preserve">/local/path/to/rev.1.2.3.fastq.gz</t>
+  </si>
+  <si>
+    <t xml:space="preserve">/local/path/to/fwd.1.2.2_2.fastq.gz</t>
+  </si>
+  <si>
+    <t xml:space="preserve">/local/path/to/rev.1.2.2_2.fastq.gz</t>
+  </si>
+  <si>
+    <t xml:space="preserve">/local/path/to/fwd.1.2.3_2.fastq.gz</t>
+  </si>
+  <si>
+    <t xml:space="preserve">/local/path/to/rev.1.2.3_2.fastq.gz</t>
   </si>
   <si>
     <t xml:space="preserve">CTTTPP124.00</t>
@@ -881,10 +863,10 @@
   <dimension ref="A1:G2013"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B11" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D37" activeCellId="0" sqref="D37"/>
+      <selection pane="topLeft" activeCell="E24" activeCellId="0" sqref="E24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.30859375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.31640625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="101" min="1" style="0" width="30.7"/>
   </cols>
@@ -1022,7 +1004,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="0" t="s">
         <v>27</v>
       </c>
@@ -1045,7 +1027,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="0" t="s">
         <v>27</v>
       </c>
@@ -1068,7 +1050,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="0" t="s">
         <v>27</v>
       </c>
@@ -1091,7 +1073,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="0" t="s">
         <v>27</v>
       </c>
@@ -1114,7 +1096,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="0" t="s">
         <v>27</v>
       </c>
@@ -1137,7 +1119,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="0" t="s">
         <v>27</v>
       </c>
@@ -1160,7 +1142,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="0" t="s">
         <v>27</v>
       </c>
@@ -1183,7 +1165,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="0" t="s">
         <v>27</v>
       </c>
@@ -1206,7 +1188,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="21" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="0" t="s">
         <v>27</v>
       </c>
@@ -1229,7 +1211,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="22" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="0" t="s">
         <v>27</v>
       </c>
@@ -1252,7 +1234,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="23" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="0" t="s">
         <v>27</v>
       </c>
@@ -1275,7 +1257,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="24" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="24" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="0" t="s">
         <v>27</v>
       </c>
@@ -1298,7 +1280,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="25" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="25" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="0" t="s">
         <v>27</v>
       </c>
@@ -1321,7 +1303,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="26" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="26" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="0" t="s">
         <v>27</v>
       </c>
@@ -1344,7 +1326,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="27" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="27" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="0" t="s">
         <v>27</v>
       </c>
@@ -1367,7 +1349,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="28" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="28" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="0" t="s">
         <v>27</v>
       </c>
@@ -1390,49 +1372,49 @@
         <v>1</v>
       </c>
     </row>
-    <row r="29" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="29" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="0" t="s">
         <v>27</v>
       </c>
-      <c r="B29" s="0" t="s">
+      <c r="B29" s="5" t="s">
         <v>74</v>
       </c>
-      <c r="C29" s="0" t="n">
+      <c r="C29" s="5" t="n">
         <v>1</v>
       </c>
-      <c r="D29" s="0" t="s">
+      <c r="D29" s="5" t="s">
         <v>75</v>
       </c>
-      <c r="E29" s="0" t="s">
+      <c r="E29" s="5" t="s">
         <v>76</v>
       </c>
       <c r="F29" s="4" t="n">
         <v>40179</v>
       </c>
-      <c r="G29" s="0" t="n">
+      <c r="G29" s="5" t="n">
         <v>1</v>
       </c>
     </row>
-    <row r="30" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="30" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="0" t="s">
         <v>27</v>
       </c>
-      <c r="B30" s="0" t="s">
+      <c r="B30" s="5" t="s">
         <v>77</v>
       </c>
-      <c r="C30" s="0" t="n">
+      <c r="C30" s="5" t="n">
         <v>1</v>
       </c>
-      <c r="D30" s="0" t="s">
+      <c r="D30" s="5" t="s">
         <v>78</v>
       </c>
-      <c r="E30" s="0" t="s">
+      <c r="E30" s="5" t="s">
         <v>79</v>
       </c>
       <c r="F30" s="4" t="n">
         <v>40179</v>
       </c>
-      <c r="G30" s="0" t="n">
+      <c r="G30" s="5" t="n">
         <v>1</v>
       </c>
     </row>
@@ -1532,49 +1514,13 @@
       <c r="A35" s="0" t="s">
         <v>27</v>
       </c>
-      <c r="B35" s="5" t="s">
-        <v>92</v>
-      </c>
-      <c r="C35" s="5" t="n">
-        <v>1</v>
-      </c>
-      <c r="D35" s="5" t="s">
-        <v>93</v>
-      </c>
-      <c r="E35" s="5" t="s">
-        <v>94</v>
-      </c>
-      <c r="F35" s="4" t="n">
-        <v>40179</v>
-      </c>
-      <c r="G35" s="5" t="n">
-        <v>1</v>
-      </c>
     </row>
     <row r="36" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="0" t="s">
         <v>27</v>
       </c>
-      <c r="B36" s="5" t="s">
-        <v>95</v>
-      </c>
-      <c r="C36" s="5" t="n">
-        <v>1</v>
-      </c>
-      <c r="D36" s="5" t="s">
-        <v>96</v>
-      </c>
-      <c r="E36" s="5" t="s">
-        <v>97</v>
-      </c>
-      <c r="F36" s="4" t="n">
-        <v>40179</v>
-      </c>
-      <c r="G36" s="5" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="37" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    </row>
+    <row r="37" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="0" t="s">
         <v>27</v>
       </c>
@@ -11485,7 +11431,7 @@
       <formula1>"Paired,Single"</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation allowBlank="true" error="Please enter date in format mm/dd/yyyy" errorStyle="stop" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="F37:F2013" type="custom">
+    <dataValidation allowBlank="true" error="Please enter date in format mm/dd/yyyy" errorStyle="stop" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="F38:F2013" type="custom">
       <formula1>AND(ISNUMBER(F27:F2026),LEFT(CELL("format",F27:F2026),1)="D")</formula1>
       <formula2>0</formula2>
     </dataValidation>
@@ -11512,19 +11458,19 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.30859375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.31640625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="101" min="2" style="0" width="30.7"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B1" s="6" t="s">
-        <v>98</v>
+        <v>92</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B2" s="1" t="s">
-        <v>99</v>
+        <v>93</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -11532,10 +11478,10 @@
         <v>3</v>
       </c>
       <c r="C3" s="0" t="s">
-        <v>100</v>
+        <v>94</v>
       </c>
       <c r="D3" s="0" t="s">
-        <v>101</v>
+        <v>95</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -11543,13 +11489,13 @@
         <v>5</v>
       </c>
       <c r="C4" s="0" t="s">
-        <v>102</v>
+        <v>96</v>
       </c>
       <c r="D4" s="0" t="s">
-        <v>103</v>
+        <v>97</v>
       </c>
       <c r="E4" s="0" t="s">
-        <v>104</v>
+        <v>98</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -11557,13 +11503,13 @@
         <v>7</v>
       </c>
       <c r="C5" s="0" t="s">
-        <v>102</v>
+        <v>96</v>
       </c>
       <c r="D5" s="0" t="s">
-        <v>105</v>
+        <v>99</v>
       </c>
       <c r="E5" s="0" t="s">
-        <v>106</v>
+        <v>100</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -11571,13 +11517,13 @@
         <v>9</v>
       </c>
       <c r="C6" s="0" t="s">
+        <v>96</v>
+      </c>
+      <c r="D6" s="0" t="s">
+        <v>101</v>
+      </c>
+      <c r="E6" s="0" t="s">
         <v>102</v>
-      </c>
-      <c r="D6" s="0" t="s">
-        <v>107</v>
-      </c>
-      <c r="E6" s="0" t="s">
-        <v>108</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -11585,13 +11531,13 @@
         <v>11</v>
       </c>
       <c r="C7" s="0" t="s">
-        <v>102</v>
+        <v>96</v>
       </c>
       <c r="D7" s="0" t="s">
-        <v>109</v>
+        <v>103</v>
       </c>
       <c r="E7" s="0" t="s">
-        <v>110</v>
+        <v>104</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -11599,13 +11545,13 @@
         <v>13</v>
       </c>
       <c r="C8" s="0" t="s">
-        <v>102</v>
+        <v>96</v>
       </c>
       <c r="D8" s="0" t="s">
-        <v>111</v>
+        <v>105</v>
       </c>
       <c r="E8" s="0" t="s">
-        <v>112</v>
+        <v>106</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -11613,10 +11559,10 @@
         <v>15</v>
       </c>
       <c r="C9" s="0" t="s">
-        <v>113</v>
+        <v>107</v>
       </c>
       <c r="D9" s="0" t="s">
-        <v>114</v>
+        <v>108</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -11624,18 +11570,18 @@
         <v>16</v>
       </c>
       <c r="C10" s="0" t="s">
-        <v>102</v>
+        <v>96</v>
       </c>
       <c r="D10" s="0" t="s">
-        <v>115</v>
+        <v>109</v>
       </c>
       <c r="E10" s="0" t="s">
-        <v>116</v>
+        <v>110</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B11" s="1" t="s">
-        <v>117</v>
+        <v>111</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -11643,13 +11589,13 @@
         <v>21</v>
       </c>
       <c r="C12" s="0" t="s">
-        <v>118</v>
+        <v>112</v>
       </c>
       <c r="D12" s="0" t="s">
-        <v>119</v>
+        <v>113</v>
       </c>
       <c r="E12" s="0" t="s">
-        <v>120</v>
+        <v>114</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -11657,7 +11603,7 @@
         <v>22</v>
       </c>
       <c r="C13" s="0" t="s">
-        <v>100</v>
+        <v>94</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -11665,10 +11611,10 @@
         <v>23</v>
       </c>
       <c r="C14" s="0" t="s">
-        <v>100</v>
+        <v>94</v>
       </c>
       <c r="D14" s="0" t="s">
-        <v>121</v>
+        <v>115</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -11676,10 +11622,10 @@
         <v>24</v>
       </c>
       <c r="C15" s="0" t="s">
-        <v>100</v>
+        <v>94</v>
       </c>
       <c r="D15" s="0" t="s">
-        <v>121</v>
+        <v>115</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -11687,10 +11633,10 @@
         <v>25</v>
       </c>
       <c r="C16" s="0" t="s">
-        <v>122</v>
+        <v>116</v>
       </c>
       <c r="D16" s="0" t="s">
-        <v>123</v>
+        <v>117</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -11698,10 +11644,10 @@
         <v>26</v>
       </c>
       <c r="C17" s="0" t="s">
-        <v>124</v>
+        <v>118</v>
       </c>
       <c r="D17" s="0" t="s">
-        <v>125</v>
+        <v>119</v>
       </c>
     </row>
   </sheetData>
@@ -11727,7 +11673,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.30859375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.31640625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="101" min="2" style="0" width="30.7"/>
   </cols>
@@ -11754,7 +11700,7 @@
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B2" s="0" t="s">
-        <v>126</v>
+        <v>120</v>
       </c>
       <c r="C2" s="0" t="s">
         <v>8</v>
@@ -11763,7 +11709,7 @@
         <v>10</v>
       </c>
       <c r="E2" s="0" t="s">
-        <v>127</v>
+        <v>121</v>
       </c>
       <c r="F2" s="0" t="s">
         <v>14</v>
@@ -11777,54 +11723,54 @@
         <v>6</v>
       </c>
       <c r="C3" s="0" t="s">
-        <v>128</v>
+        <v>122</v>
       </c>
       <c r="D3" s="0" t="s">
-        <v>129</v>
+        <v>123</v>
       </c>
       <c r="E3" s="0" t="s">
-        <v>130</v>
+        <v>124</v>
       </c>
       <c r="F3" s="0" t="s">
-        <v>131</v>
+        <v>125</v>
       </c>
       <c r="G3" s="0" t="s">
-        <v>132</v>
+        <v>126</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B4" s="0" t="s">
-        <v>133</v>
+        <v>127</v>
       </c>
       <c r="D4" s="0" t="s">
-        <v>134</v>
+        <v>128</v>
       </c>
       <c r="E4" s="0" t="s">
         <v>12</v>
       </c>
       <c r="G4" s="0" t="s">
-        <v>135</v>
+        <v>129</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B5" s="0" t="s">
-        <v>136</v>
+        <v>130</v>
       </c>
       <c r="D5" s="0" t="s">
-        <v>137</v>
+        <v>131</v>
       </c>
       <c r="E5" s="0" t="s">
-        <v>138</v>
+        <v>132</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E6" s="0" t="s">
-        <v>139</v>
+        <v>133</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E7" s="0" t="s">
-        <v>140</v>
+        <v>134</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
CIDC-1508 bucket names, cimac_center
</commit_message>
<xml_diff>
--- a/template_examples/wes_fastq_template.xlsx
+++ b/template_examples/wes_fastq_template.xlsx
@@ -236,354 +236,357 @@
     <t xml:space="preserve">Assay creator</t>
   </si>
   <si>
+    <t xml:space="preserve">MD Anderson</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sequencing protocol</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Express Somatic Human WES (Deep Coverage) v1.1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Library kit</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Hyper Prep ICE Exome Express: 1.0</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sequencer platform</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Illumina - NextSeq 550</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Paired end reads</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Paired</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Read length</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Bait set</t>
+  </si>
+  <si>
+    <t xml:space="preserve">whole_exome_illumina_coding_v1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">#skip</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Samples</t>
+  </si>
+  <si>
+    <t xml:space="preserve">#header</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Cimac id</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Lane</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Forward fastq</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Reverse fastq</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sequencing date</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Quality flag</t>
+  </si>
+  <si>
+    <t xml:space="preserve">#data</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CTTTPP122.00</t>
+  </si>
+  <si>
+    <t xml:space="preserve">/local/path/to/fwd.1.2.2.fastq.gz</t>
+  </si>
+  <si>
+    <t xml:space="preserve">/local/path/to/rev.1.2.2.fastq.gz</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CTTTPP123.00</t>
+  </si>
+  <si>
+    <t xml:space="preserve">/local/path/to/fwd.1.2.3.fastq.gz</t>
+  </si>
+  <si>
+    <t xml:space="preserve">/local/path/to/rev.1.2.3.fastq.gz</t>
+  </si>
+  <si>
+    <t xml:space="preserve">/local/path/to/fwd.1.2.2_2.fastq.gz</t>
+  </si>
+  <si>
+    <t xml:space="preserve">/local/path/to/rev.1.2.2_2.fastq.gz</t>
+  </si>
+  <si>
+    <t xml:space="preserve">/local/path/to/fwd.1.2.3_2.fastq.gz</t>
+  </si>
+  <si>
+    <t xml:space="preserve">/local/path/to/rev.1.2.3_2.fastq.gz</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CTTTPP124.00</t>
+  </si>
+  <si>
+    <t xml:space="preserve">/local/path/to/fwd.1.2.4.fastq.gz</t>
+  </si>
+  <si>
+    <t xml:space="preserve">/local/path/to/rev.1.2.4.fastq.gz</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CTTTPP211.00</t>
+  </si>
+  <si>
+    <t xml:space="preserve">/local/path/to/fwd.2.1.1.fastq.gz</t>
+  </si>
+  <si>
+    <t xml:space="preserve">/local/path/to/rev.2.1.1.fastq.gz</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CTTTPP212.00</t>
+  </si>
+  <si>
+    <t xml:space="preserve">/local/path/to/fwd.2.1.2.fastq.gz</t>
+  </si>
+  <si>
+    <t xml:space="preserve">/local/path/to/rev.2.1.2.fastq.gz</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CTTTPP213.00</t>
+  </si>
+  <si>
+    <t xml:space="preserve">/local/path/to/fwd.2.1.3.fastq.gz</t>
+  </si>
+  <si>
+    <t xml:space="preserve">/local/path/to/rev.2.1.3.fastq.gz</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CTTTPP214.00</t>
+  </si>
+  <si>
+    <t xml:space="preserve">/local/path/to/fwd.2.1.4.fastq.gz</t>
+  </si>
+  <si>
+    <t xml:space="preserve">/local/path/to/rev.2.1.4.fastq.gz</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CTTTPP311.00</t>
+  </si>
+  <si>
+    <t xml:space="preserve">/local/path/to/fwd.3.1.1.fastq.gz</t>
+  </si>
+  <si>
+    <t xml:space="preserve">/local/path/to/rev.3.1.1.fastq.gz</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CTTTPP312.00</t>
+  </si>
+  <si>
+    <t xml:space="preserve">/local/path/to/fwd.3.1.2.fastq.gz</t>
+  </si>
+  <si>
+    <t xml:space="preserve">/local/path/to/rev.3.1.2.fastq.gz</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CTTTPP313.00</t>
+  </si>
+  <si>
+    <t xml:space="preserve">/local/path/to/fwd.3.1.3.fastq.gz</t>
+  </si>
+  <si>
+    <t xml:space="preserve">/local/path/to/rev.3.1.3.fastq.gz</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CTTTPP411.00</t>
+  </si>
+  <si>
+    <t xml:space="preserve">/local/path/to/fwd.4.1.1.fastq.gz</t>
+  </si>
+  <si>
+    <t xml:space="preserve">/local/path/to/rev.4.1.1.fastq.gz</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CTTTPP412.00</t>
+  </si>
+  <si>
+    <t xml:space="preserve">/local/path/to/fwd.4.1.2.fastq.gz</t>
+  </si>
+  <si>
+    <t xml:space="preserve">/local/path/to/rev.4.1.2.fastq.gz</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CTTTPP413.00</t>
+  </si>
+  <si>
+    <t xml:space="preserve">/local/path/to/fwd.4.1.3.fastq.gz</t>
+  </si>
+  <si>
+    <t xml:space="preserve">/local/path/to/rev.4.1.3.fastq.gz</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CTTTPP511.00</t>
+  </si>
+  <si>
+    <t xml:space="preserve">/local/path/to/fwd.5.1.1.fastq.gz</t>
+  </si>
+  <si>
+    <t xml:space="preserve">/local/path/to/rev.5.1.1.fastq.gz</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CTTTPP512.00</t>
+  </si>
+  <si>
+    <t xml:space="preserve">/local/path/to/fwd.5.1.2.fastq.gz</t>
+  </si>
+  <si>
+    <t xml:space="preserve">/local/path/to/rev.5.1.2.fastq.gz</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CTTTPP513.00</t>
+  </si>
+  <si>
+    <t xml:space="preserve">/local/path/to/fwd.5.1.3.fastq.gz</t>
+  </si>
+  <si>
+    <t xml:space="preserve">/local/path/to/rev.5.1.3.fastq.gz</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CTTTPP514.00</t>
+  </si>
+  <si>
+    <t xml:space="preserve">/local/path/to/fwd.5.1.4.fastq.gz</t>
+  </si>
+  <si>
+    <t xml:space="preserve">/local/path/to/rev.5.1.4.fastq.gz</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CTTTPP515.00</t>
+  </si>
+  <si>
+    <t xml:space="preserve">/local/path/to/fwd.5.1.5.fastq.gz</t>
+  </si>
+  <si>
+    <t xml:space="preserve">/local/path/to/rev.5.1.5.fastq.gz</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CTTTPP516.00</t>
+  </si>
+  <si>
+    <t xml:space="preserve">/local/path/to/fwd.5.1.6.fastq.gz</t>
+  </si>
+  <si>
+    <t xml:space="preserve">/local/path/to/rev.5.1.6.fastq.gz</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CTTTPP517.00</t>
+  </si>
+  <si>
+    <t xml:space="preserve">/local/path/to/fwd.5.1.7.fastq.gz</t>
+  </si>
+  <si>
+    <t xml:space="preserve">/local/path/to/rev.5.1.7.fastq.gz</t>
+  </si>
+  <si>
+    <t xml:space="preserve">LEGEND</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Legend for tab 'WES'</t>
+  </si>
+  <si>
+    <t xml:space="preserve">String</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Trial identifier used by lead organization, ie. Center for Experimental Therapeutics Program (CTEP) ID or Industry Sponsored ID.  This is usually a short identifier. Example: E4412.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Enum</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Indicates what site is filling out the assay.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">E.g. 'DFCI'</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Protocol and version used for the sequencing.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">E.g. 'Express Somatic Human WES (Deep Coverage) v1.1'</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The library construction kit.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">E.g. 'Hyper Prep ICE Exome Express: 1.0'</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sequencer Model, e.g. HiSeq 2500, NextSeq, NovaSeq.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">E.g. 'Illumina - HiSeq 2500'</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Indicates if the sequencing was performed paired or single ended.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">E.g. 'Paired'</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Integer</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Number of cycles for each sequencing read.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Bait set ID.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">E.g. 'whole_exome_illumina_coding_v1'</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Section 'Samples' of tab 'WES'</t>
+  </si>
+  <si>
+    <t xml:space="preserve">String: regex ^C[A-Z0-9]{3}[A-Z0-9]{3}[A-Z0-9]{2}.[0-9]{2}$ </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Specimen identifier assigned by the CIMAC-CIDC Network. Formatted as C????????.??</t>
+  </si>
+  <si>
+    <t xml:space="preserve">E.g. 'CTTTP01A1.00'</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Path to a file on a user's computer.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">String: date </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Date of sequencing.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Number</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Flag used for quality.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DFCI</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Illumina - HiSeq 2500</t>
+  </si>
+  <si>
     <t xml:space="preserve">Mount Sinai</t>
   </si>
   <si>
-    <t xml:space="preserve">Sequencing protocol</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Express Somatic Human WES (Deep Coverage) v1.1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Library kit</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Hyper Prep ICE Exome Express: 1.0</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Sequencer platform</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Illumina - NextSeq 550</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Paired end reads</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Paired</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Read length</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Bait set</t>
-  </si>
-  <si>
-    <t xml:space="preserve">whole_exome_illumina_coding_v1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">#skip</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Samples</t>
-  </si>
-  <si>
-    <t xml:space="preserve">#header</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Cimac id</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Lane</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Forward fastq</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Reverse fastq</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Sequencing date</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Quality flag</t>
-  </si>
-  <si>
-    <t xml:space="preserve">#data</t>
-  </si>
-  <si>
-    <t xml:space="preserve">CTTTPP122.00</t>
-  </si>
-  <si>
-    <t xml:space="preserve">/local/path/to/fwd.1.2.2.fastq.gz</t>
-  </si>
-  <si>
-    <t xml:space="preserve">/local/path/to/rev.1.2.2.fastq.gz</t>
-  </si>
-  <si>
-    <t xml:space="preserve">CTTTPP123.00</t>
-  </si>
-  <si>
-    <t xml:space="preserve">/local/path/to/fwd.1.2.3.fastq.gz</t>
-  </si>
-  <si>
-    <t xml:space="preserve">/local/path/to/rev.1.2.3.fastq.gz</t>
-  </si>
-  <si>
-    <t xml:space="preserve">/local/path/to/fwd.1.2.2_2.fastq.gz</t>
-  </si>
-  <si>
-    <t xml:space="preserve">/local/path/to/rev.1.2.2_2.fastq.gz</t>
-  </si>
-  <si>
-    <t xml:space="preserve">/local/path/to/fwd.1.2.3_2.fastq.gz</t>
-  </si>
-  <si>
-    <t xml:space="preserve">/local/path/to/rev.1.2.3_2.fastq.gz</t>
-  </si>
-  <si>
-    <t xml:space="preserve">CTTTPP124.00</t>
-  </si>
-  <si>
-    <t xml:space="preserve">/local/path/to/fwd.1.2.4.fastq.gz</t>
-  </si>
-  <si>
-    <t xml:space="preserve">/local/path/to/rev.1.2.4.fastq.gz</t>
-  </si>
-  <si>
-    <t xml:space="preserve">CTTTPP211.00</t>
-  </si>
-  <si>
-    <t xml:space="preserve">/local/path/to/fwd.2.1.1.fastq.gz</t>
-  </si>
-  <si>
-    <t xml:space="preserve">/local/path/to/rev.2.1.1.fastq.gz</t>
-  </si>
-  <si>
-    <t xml:space="preserve">CTTTPP212.00</t>
-  </si>
-  <si>
-    <t xml:space="preserve">/local/path/to/fwd.2.1.2.fastq.gz</t>
-  </si>
-  <si>
-    <t xml:space="preserve">/local/path/to/rev.2.1.2.fastq.gz</t>
-  </si>
-  <si>
-    <t xml:space="preserve">CTTTPP213.00</t>
-  </si>
-  <si>
-    <t xml:space="preserve">/local/path/to/fwd.2.1.3.fastq.gz</t>
-  </si>
-  <si>
-    <t xml:space="preserve">/local/path/to/rev.2.1.3.fastq.gz</t>
-  </si>
-  <si>
-    <t xml:space="preserve">CTTTPP214.00</t>
-  </si>
-  <si>
-    <t xml:space="preserve">/local/path/to/fwd.2.1.4.fastq.gz</t>
-  </si>
-  <si>
-    <t xml:space="preserve">/local/path/to/rev.2.1.4.fastq.gz</t>
-  </si>
-  <si>
-    <t xml:space="preserve">CTTTPP311.00</t>
-  </si>
-  <si>
-    <t xml:space="preserve">/local/path/to/fwd.3.1.1.fastq.gz</t>
-  </si>
-  <si>
-    <t xml:space="preserve">/local/path/to/rev.3.1.1.fastq.gz</t>
-  </si>
-  <si>
-    <t xml:space="preserve">CTTTPP312.00</t>
-  </si>
-  <si>
-    <t xml:space="preserve">/local/path/to/fwd.3.1.2.fastq.gz</t>
-  </si>
-  <si>
-    <t xml:space="preserve">/local/path/to/rev.3.1.2.fastq.gz</t>
-  </si>
-  <si>
-    <t xml:space="preserve">CTTTPP313.00</t>
-  </si>
-  <si>
-    <t xml:space="preserve">/local/path/to/fwd.3.1.3.fastq.gz</t>
-  </si>
-  <si>
-    <t xml:space="preserve">/local/path/to/rev.3.1.3.fastq.gz</t>
-  </si>
-  <si>
-    <t xml:space="preserve">CTTTPP411.00</t>
-  </si>
-  <si>
-    <t xml:space="preserve">/local/path/to/fwd.4.1.1.fastq.gz</t>
-  </si>
-  <si>
-    <t xml:space="preserve">/local/path/to/rev.4.1.1.fastq.gz</t>
-  </si>
-  <si>
-    <t xml:space="preserve">CTTTPP412.00</t>
-  </si>
-  <si>
-    <t xml:space="preserve">/local/path/to/fwd.4.1.2.fastq.gz</t>
-  </si>
-  <si>
-    <t xml:space="preserve">/local/path/to/rev.4.1.2.fastq.gz</t>
-  </si>
-  <si>
-    <t xml:space="preserve">CTTTPP413.00</t>
-  </si>
-  <si>
-    <t xml:space="preserve">/local/path/to/fwd.4.1.3.fastq.gz</t>
-  </si>
-  <si>
-    <t xml:space="preserve">/local/path/to/rev.4.1.3.fastq.gz</t>
-  </si>
-  <si>
-    <t xml:space="preserve">CTTTPP511.00</t>
-  </si>
-  <si>
-    <t xml:space="preserve">/local/path/to/fwd.5.1.1.fastq.gz</t>
-  </si>
-  <si>
-    <t xml:space="preserve">/local/path/to/rev.5.1.1.fastq.gz</t>
-  </si>
-  <si>
-    <t xml:space="preserve">CTTTPP512.00</t>
-  </si>
-  <si>
-    <t xml:space="preserve">/local/path/to/fwd.5.1.2.fastq.gz</t>
-  </si>
-  <si>
-    <t xml:space="preserve">/local/path/to/rev.5.1.2.fastq.gz</t>
-  </si>
-  <si>
-    <t xml:space="preserve">CTTTPP513.00</t>
-  </si>
-  <si>
-    <t xml:space="preserve">/local/path/to/fwd.5.1.3.fastq.gz</t>
-  </si>
-  <si>
-    <t xml:space="preserve">/local/path/to/rev.5.1.3.fastq.gz</t>
-  </si>
-  <si>
-    <t xml:space="preserve">CTTTPP514.00</t>
-  </si>
-  <si>
-    <t xml:space="preserve">/local/path/to/fwd.5.1.4.fastq.gz</t>
-  </si>
-  <si>
-    <t xml:space="preserve">/local/path/to/rev.5.1.4.fastq.gz</t>
-  </si>
-  <si>
-    <t xml:space="preserve">CTTTPP515.00</t>
-  </si>
-  <si>
-    <t xml:space="preserve">/local/path/to/fwd.5.1.5.fastq.gz</t>
-  </si>
-  <si>
-    <t xml:space="preserve">/local/path/to/rev.5.1.5.fastq.gz</t>
-  </si>
-  <si>
-    <t xml:space="preserve">CTTTPP516.00</t>
-  </si>
-  <si>
-    <t xml:space="preserve">/local/path/to/fwd.5.1.6.fastq.gz</t>
-  </si>
-  <si>
-    <t xml:space="preserve">/local/path/to/rev.5.1.6.fastq.gz</t>
-  </si>
-  <si>
-    <t xml:space="preserve">CTTTPP517.00</t>
-  </si>
-  <si>
-    <t xml:space="preserve">/local/path/to/fwd.5.1.7.fastq.gz</t>
-  </si>
-  <si>
-    <t xml:space="preserve">/local/path/to/rev.5.1.7.fastq.gz</t>
-  </si>
-  <si>
-    <t xml:space="preserve">LEGEND</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Legend for tab 'WES'</t>
-  </si>
-  <si>
-    <t xml:space="preserve">String</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Trial identifier used by lead organization, ie. Center for Experimental Therapeutics Program (CTEP) ID or Industry Sponsored ID.  This is usually a short identifier. Example: E4412.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Enum</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Indicates what site is filling out the assay.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">E.g. 'DFCI'</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Protocol and version used for the sequencing.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">E.g. 'Express Somatic Human WES (Deep Coverage) v1.1'</t>
-  </si>
-  <si>
-    <t xml:space="preserve">The library construction kit.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">E.g. 'Hyper Prep ICE Exome Express: 1.0'</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Sequencer Model, e.g. HiSeq 2500, NextSeq, NovaSeq.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">E.g. 'Illumina - HiSeq 2500'</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Indicates if the sequencing was performed paired or single ended.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">E.g. 'Paired'</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Integer</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Number of cycles for each sequencing read.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Bait set ID.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">E.g. 'whole_exome_illumina_coding_v1'</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Section 'Samples' of tab 'WES'</t>
-  </si>
-  <si>
-    <t xml:space="preserve">String: regex ^C[A-Z0-9]{3}[A-Z0-9]{3}[A-Z0-9]{2}.[0-9]{2}$ </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Specimen identifier assigned by the CIMAC-CIDC Network. Formatted as C????????.??</t>
-  </si>
-  <si>
-    <t xml:space="preserve">E.g. 'CTTTP01A1.00'</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Path to a file on a user's computer.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">String: date </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Date of sequencing.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Number</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Flag used for quality.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">DFCI</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Illumina - HiSeq 2500</t>
-  </si>
-  <si>
     <t xml:space="preserve">Somatic Human WES v6</t>
   </si>
   <si>
@@ -606,9 +609,6 @@
   </si>
   <si>
     <t xml:space="preserve">TWIST Dana Farber Custom Panel</t>
-  </si>
-  <si>
-    <t xml:space="preserve">MD Anderson</t>
   </si>
   <si>
     <t xml:space="preserve">TWIST</t>
@@ -862,11 +862,11 @@
   </sheetPr>
   <dimension ref="A1:G2013"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B11" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E24" activeCellId="0" sqref="E24"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C3" activeCellId="0" sqref="C3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.31640625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.328125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="101" min="1" style="0" width="30.7"/>
   </cols>
@@ -891,7 +891,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
         <v>2</v>
       </c>
@@ -11458,7 +11458,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.31640625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.328125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="101" min="2" style="0" width="30.7"/>
   </cols>
@@ -11673,7 +11673,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.31640625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.328125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="101" min="2" style="0" width="30.7"/>
   </cols>
@@ -11720,41 +11720,41 @@
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B3" s="0" t="s">
-        <v>6</v>
+        <v>122</v>
       </c>
       <c r="C3" s="0" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="D3" s="0" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="E3" s="0" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="F3" s="0" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="G3" s="0" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B4" s="0" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="D4" s="0" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="E4" s="0" t="s">
         <v>12</v>
       </c>
       <c r="G4" s="0" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B5" s="0" t="s">
-        <v>130</v>
+        <v>6</v>
       </c>
       <c r="D5" s="0" t="s">
         <v>131</v>

</xml_diff>

<commit_message>
CIDC-1533 tumor-normal pairing csv update
</commit_message>
<xml_diff>
--- a/template_examples/wes_fastq_template.xlsx
+++ b/template_examples/wes_fastq_template.xlsx
@@ -216,7 +216,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2186" uniqueCount="140">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2189" uniqueCount="143">
   <si>
     <t xml:space="preserve">#title</t>
   </si>
@@ -492,6 +492,15 @@
   </si>
   <si>
     <t xml:space="preserve">/local/path/to/rev.5.1.7.fastq.gz</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CTTTPP518.00</t>
+  </si>
+  <si>
+    <t xml:space="preserve">/local/path/to/fwd.5.1.8.fastq.gz</t>
+  </si>
+  <si>
+    <t xml:space="preserve">/local/path/to/rev.5.1.8.fastq.gz</t>
   </si>
   <si>
     <t xml:space="preserve">LEGEND</t>
@@ -877,11 +886,11 @@
   </sheetPr>
   <dimension ref="A1:G2012"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B13" activeCellId="0" sqref="B13:G34"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="G18" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B36" activeCellId="0" sqref="B36:G36"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.28125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.30859375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="101" min="1" style="0" width="30.7"/>
   </cols>
@@ -1525,15 +1534,39 @@
         <v>1</v>
       </c>
     </row>
-    <row r="35" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="35" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="0" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="36" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B35" s="4" t="s">
+        <v>92</v>
+      </c>
+      <c r="C35" s="4" t="n">
+        <v>1</v>
+      </c>
+      <c r="D35" s="4" t="s">
+        <v>93</v>
+      </c>
+      <c r="E35" s="4" t="s">
+        <v>94</v>
+      </c>
+      <c r="F35" s="5" t="n">
+        <v>40179</v>
+      </c>
+      <c r="G35" s="4" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="36" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="0" t="s">
         <v>27</v>
       </c>
+      <c r="B36" s="4"/>
+      <c r="C36" s="4"/>
+      <c r="D36" s="4"/>
+      <c r="E36" s="4"/>
+      <c r="F36" s="5"/>
+      <c r="G36" s="4"/>
     </row>
     <row r="37" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="0" t="s">
@@ -11421,7 +11454,7 @@
     <mergeCell ref="B11:G11"/>
   </mergeCells>
   <dataValidations count="6">
-    <dataValidation allowBlank="true" error="Please enter date in format mm/dd/yyyy" errorStyle="stop" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="F35:F2012" type="custom">
+    <dataValidation allowBlank="true" error="Please enter date in format mm/dd/yyyy" errorStyle="stop" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="F37:F2012" type="custom">
       <formula1>AND(ISNUMBER(F13:F2012),LEFT(CELL("format",F13:F2012),1)="D")</formula1>
       <formula2>0</formula2>
     </dataValidation>
@@ -11465,22 +11498,22 @@
   <dimension ref="B1:E17"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="1" sqref="B13:G34 A1"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="1" sqref="B36:G36 A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.28125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.30859375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="101" min="2" style="0" width="30.7"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B1" s="6" t="s">
-        <v>92</v>
+        <v>95</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B2" s="1" t="s">
-        <v>93</v>
+        <v>96</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -11488,10 +11521,10 @@
         <v>3</v>
       </c>
       <c r="C3" s="0" t="s">
-        <v>94</v>
+        <v>97</v>
       </c>
       <c r="D3" s="0" t="s">
-        <v>95</v>
+        <v>98</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -11499,13 +11532,13 @@
         <v>5</v>
       </c>
       <c r="C4" s="0" t="s">
-        <v>96</v>
+        <v>99</v>
       </c>
       <c r="D4" s="0" t="s">
-        <v>97</v>
+        <v>100</v>
       </c>
       <c r="E4" s="0" t="s">
-        <v>98</v>
+        <v>101</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -11513,13 +11546,13 @@
         <v>7</v>
       </c>
       <c r="C5" s="0" t="s">
-        <v>96</v>
+        <v>99</v>
       </c>
       <c r="D5" s="0" t="s">
-        <v>99</v>
+        <v>102</v>
       </c>
       <c r="E5" s="0" t="s">
-        <v>100</v>
+        <v>103</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -11527,13 +11560,13 @@
         <v>9</v>
       </c>
       <c r="C6" s="0" t="s">
-        <v>96</v>
+        <v>99</v>
       </c>
       <c r="D6" s="0" t="s">
-        <v>101</v>
+        <v>104</v>
       </c>
       <c r="E6" s="0" t="s">
-        <v>102</v>
+        <v>105</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -11541,13 +11574,13 @@
         <v>11</v>
       </c>
       <c r="C7" s="0" t="s">
-        <v>96</v>
+        <v>99</v>
       </c>
       <c r="D7" s="0" t="s">
-        <v>103</v>
+        <v>106</v>
       </c>
       <c r="E7" s="0" t="s">
-        <v>104</v>
+        <v>107</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -11555,13 +11588,13 @@
         <v>13</v>
       </c>
       <c r="C8" s="0" t="s">
-        <v>96</v>
+        <v>99</v>
       </c>
       <c r="D8" s="0" t="s">
-        <v>105</v>
+        <v>108</v>
       </c>
       <c r="E8" s="0" t="s">
-        <v>106</v>
+        <v>109</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -11569,10 +11602,10 @@
         <v>15</v>
       </c>
       <c r="C9" s="0" t="s">
-        <v>107</v>
+        <v>110</v>
       </c>
       <c r="D9" s="0" t="s">
-        <v>108</v>
+        <v>111</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -11580,18 +11613,18 @@
         <v>16</v>
       </c>
       <c r="C10" s="0" t="s">
-        <v>96</v>
+        <v>99</v>
       </c>
       <c r="D10" s="0" t="s">
-        <v>109</v>
+        <v>112</v>
       </c>
       <c r="E10" s="0" t="s">
-        <v>110</v>
+        <v>113</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B11" s="1" t="s">
-        <v>111</v>
+        <v>114</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -11599,13 +11632,13 @@
         <v>21</v>
       </c>
       <c r="C12" s="0" t="s">
-        <v>112</v>
+        <v>115</v>
       </c>
       <c r="D12" s="0" t="s">
-        <v>113</v>
+        <v>116</v>
       </c>
       <c r="E12" s="0" t="s">
-        <v>114</v>
+        <v>117</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -11613,7 +11646,7 @@
         <v>22</v>
       </c>
       <c r="C13" s="0" t="s">
-        <v>94</v>
+        <v>97</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -11621,10 +11654,10 @@
         <v>23</v>
       </c>
       <c r="C14" s="0" t="s">
-        <v>94</v>
+        <v>97</v>
       </c>
       <c r="D14" s="0" t="s">
-        <v>115</v>
+        <v>118</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -11632,10 +11665,10 @@
         <v>24</v>
       </c>
       <c r="C15" s="0" t="s">
-        <v>94</v>
+        <v>97</v>
       </c>
       <c r="D15" s="0" t="s">
-        <v>115</v>
+        <v>118</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -11643,10 +11676,10 @@
         <v>25</v>
       </c>
       <c r="C16" s="0" t="s">
-        <v>116</v>
+        <v>119</v>
       </c>
       <c r="D16" s="0" t="s">
-        <v>117</v>
+        <v>120</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -11654,10 +11687,10 @@
         <v>26</v>
       </c>
       <c r="C17" s="0" t="s">
-        <v>118</v>
+        <v>121</v>
       </c>
       <c r="D17" s="0" t="s">
-        <v>119</v>
+        <v>122</v>
       </c>
     </row>
   </sheetData>
@@ -11680,10 +11713,10 @@
   <dimension ref="B1:G8"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="1" sqref="B13:G34 A1"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="1" sqref="B36:G36 A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.28125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.30859375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="101" min="2" style="0" width="30.7"/>
   </cols>
@@ -11710,7 +11743,7 @@
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B2" s="0" t="s">
-        <v>120</v>
+        <v>123</v>
       </c>
       <c r="C2" s="0" t="s">
         <v>8</v>
@@ -11719,7 +11752,7 @@
         <v>10</v>
       </c>
       <c r="E2" s="0" t="s">
-        <v>121</v>
+        <v>124</v>
       </c>
       <c r="F2" s="0" t="s">
         <v>14</v>
@@ -11730,39 +11763,39 @@
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B3" s="0" t="s">
-        <v>122</v>
+        <v>125</v>
       </c>
       <c r="C3" s="0" t="s">
-        <v>123</v>
+        <v>126</v>
       </c>
       <c r="D3" s="0" t="s">
-        <v>124</v>
+        <v>127</v>
       </c>
       <c r="E3" s="0" t="s">
-        <v>125</v>
+        <v>128</v>
       </c>
       <c r="F3" s="0" t="s">
-        <v>126</v>
+        <v>129</v>
       </c>
       <c r="G3" s="0" t="s">
-        <v>127</v>
+        <v>130</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B4" s="0" t="s">
-        <v>128</v>
+        <v>131</v>
       </c>
       <c r="C4" s="0" t="s">
-        <v>129</v>
+        <v>132</v>
       </c>
       <c r="D4" s="0" t="s">
-        <v>130</v>
+        <v>133</v>
       </c>
       <c r="E4" s="0" t="s">
-        <v>131</v>
+        <v>134</v>
       </c>
       <c r="G4" s="0" t="s">
-        <v>132</v>
+        <v>135</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -11770,43 +11803,43 @@
         <v>6</v>
       </c>
       <c r="C5" s="0" t="s">
-        <v>133</v>
+        <v>136</v>
       </c>
       <c r="D5" s="0" t="s">
-        <v>134</v>
+        <v>137</v>
       </c>
       <c r="E5" s="0" t="s">
         <v>12</v>
       </c>
       <c r="G5" s="0" t="s">
-        <v>129</v>
+        <v>132</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B6" s="0" t="s">
-        <v>121</v>
+        <v>124</v>
       </c>
       <c r="D6" s="0" t="s">
-        <v>133</v>
+        <v>136</v>
       </c>
       <c r="E6" s="0" t="s">
-        <v>135</v>
+        <v>138</v>
       </c>
       <c r="G6" s="0" t="s">
-        <v>136</v>
+        <v>139</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B7" s="0" t="s">
-        <v>137</v>
+        <v>140</v>
       </c>
       <c r="E7" s="0" t="s">
-        <v>138</v>
+        <v>141</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E8" s="0" t="s">
-        <v>139</v>
+        <v>142</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
CIDC-1544 add records to example template
</commit_message>
<xml_diff>
--- a/template_examples/wes_fastq_template.xlsx
+++ b/template_examples/wes_fastq_template.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl$\Ubuntu-20.04\home\jamesp\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl$\Ubuntu-20.04\home\jamesp\cidc-schemas\template_examples\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2E50FF02-DCC0-4066-A670-028F6F7A4D37}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0DC79326-A447-422A-85CC-24A19AA2E6E3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="21090" yWindow="1200" windowWidth="20355" windowHeight="10920" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="WES" sheetId="1" r:id="rId1"/>
@@ -203,7 +203,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2120" uniqueCount="76">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2189" uniqueCount="143">
   <si>
     <t>LEGEND</t>
   </si>
@@ -431,6 +431,207 @@
   </si>
   <si>
     <t>test_prism_trial_id</t>
+  </si>
+  <si>
+    <t>CTTTPP122.00</t>
+  </si>
+  <si>
+    <t>/local/path/to/fwd.1.2.2.fastq.gz</t>
+  </si>
+  <si>
+    <t>/local/path/to/rev.1.2.2.fastq.gz</t>
+  </si>
+  <si>
+    <t>CTTTPP123.00</t>
+  </si>
+  <si>
+    <t>/local/path/to/fwd.1.2.3.fastq.gz</t>
+  </si>
+  <si>
+    <t>/local/path/to/rev.1.2.3.fastq.gz</t>
+  </si>
+  <si>
+    <t>/local/path/to/fwd.1.2.2_2.fastq.gz</t>
+  </si>
+  <si>
+    <t>/local/path/to/rev.1.2.2_2.fastq.gz</t>
+  </si>
+  <si>
+    <t>/local/path/to/fwd.1.2.3_2.fastq.gz</t>
+  </si>
+  <si>
+    <t>/local/path/to/rev.1.2.3_2.fastq.gz</t>
+  </si>
+  <si>
+    <t>CTTTPP124.00</t>
+  </si>
+  <si>
+    <t>/local/path/to/fwd.1.2.4.fastq.gz</t>
+  </si>
+  <si>
+    <t>/local/path/to/rev.1.2.4.fastq.gz</t>
+  </si>
+  <si>
+    <t>CTTTPP211.00</t>
+  </si>
+  <si>
+    <t>/local/path/to/fwd.2.1.1.fastq.gz</t>
+  </si>
+  <si>
+    <t>/local/path/to/rev.2.1.1.fastq.gz</t>
+  </si>
+  <si>
+    <t>CTTTPP212.00</t>
+  </si>
+  <si>
+    <t>/local/path/to/fwd.2.1.2.fastq.gz</t>
+  </si>
+  <si>
+    <t>/local/path/to/rev.2.1.2.fastq.gz</t>
+  </si>
+  <si>
+    <t>CTTTPP213.00</t>
+  </si>
+  <si>
+    <t>/local/path/to/fwd.2.1.3.fastq.gz</t>
+  </si>
+  <si>
+    <t>/local/path/to/rev.2.1.3.fastq.gz</t>
+  </si>
+  <si>
+    <t>CTTTPP214.00</t>
+  </si>
+  <si>
+    <t>/local/path/to/fwd.2.1.4.fastq.gz</t>
+  </si>
+  <si>
+    <t>/local/path/to/rev.2.1.4.fastq.gz</t>
+  </si>
+  <si>
+    <t>CTTTPP311.00</t>
+  </si>
+  <si>
+    <t>/local/path/to/fwd.3.1.1.fastq.gz</t>
+  </si>
+  <si>
+    <t>/local/path/to/rev.3.1.1.fastq.gz</t>
+  </si>
+  <si>
+    <t>CTTTPP312.00</t>
+  </si>
+  <si>
+    <t>/local/path/to/fwd.3.1.2.fastq.gz</t>
+  </si>
+  <si>
+    <t>/local/path/to/rev.3.1.2.fastq.gz</t>
+  </si>
+  <si>
+    <t>CTTTPP313.00</t>
+  </si>
+  <si>
+    <t>/local/path/to/fwd.3.1.3.fastq.gz</t>
+  </si>
+  <si>
+    <t>/local/path/to/rev.3.1.3.fastq.gz</t>
+  </si>
+  <si>
+    <t>CTTTPP411.00</t>
+  </si>
+  <si>
+    <t>/local/path/to/fwd.4.1.1.fastq.gz</t>
+  </si>
+  <si>
+    <t>/local/path/to/rev.4.1.1.fastq.gz</t>
+  </si>
+  <si>
+    <t>CTTTPP412.00</t>
+  </si>
+  <si>
+    <t>/local/path/to/fwd.4.1.2.fastq.gz</t>
+  </si>
+  <si>
+    <t>/local/path/to/rev.4.1.2.fastq.gz</t>
+  </si>
+  <si>
+    <t>CTTTPP413.00</t>
+  </si>
+  <si>
+    <t>/local/path/to/fwd.4.1.3.fastq.gz</t>
+  </si>
+  <si>
+    <t>/local/path/to/rev.4.1.3.fastq.gz</t>
+  </si>
+  <si>
+    <t>CTTTPP511.00</t>
+  </si>
+  <si>
+    <t>/local/path/to/fwd.5.1.1.fastq.gz</t>
+  </si>
+  <si>
+    <t>/local/path/to/rev.5.1.1.fastq.gz</t>
+  </si>
+  <si>
+    <t>CTTTPP512.00</t>
+  </si>
+  <si>
+    <t>/local/path/to/fwd.5.1.2.fastq.gz</t>
+  </si>
+  <si>
+    <t>/local/path/to/rev.5.1.2.fastq.gz</t>
+  </si>
+  <si>
+    <t>CTTTPP513.00</t>
+  </si>
+  <si>
+    <t>/local/path/to/fwd.5.1.3.fastq.gz</t>
+  </si>
+  <si>
+    <t>/local/path/to/rev.5.1.3.fastq.gz</t>
+  </si>
+  <si>
+    <t>CTTTPP514.00</t>
+  </si>
+  <si>
+    <t>/local/path/to/fwd.5.1.4.fastq.gz</t>
+  </si>
+  <si>
+    <t>/local/path/to/rev.5.1.4.fastq.gz</t>
+  </si>
+  <si>
+    <t>CTTTPP515.00</t>
+  </si>
+  <si>
+    <t>/local/path/to/fwd.5.1.5.fastq.gz</t>
+  </si>
+  <si>
+    <t>/local/path/to/rev.5.1.5.fastq.gz</t>
+  </si>
+  <si>
+    <t>CTTTPP516.00</t>
+  </si>
+  <si>
+    <t>/local/path/to/fwd.5.1.6.fastq.gz</t>
+  </si>
+  <si>
+    <t>/local/path/to/rev.5.1.6.fastq.gz</t>
+  </si>
+  <si>
+    <t>CTTTPP517.00</t>
+  </si>
+  <si>
+    <t>/local/path/to/fwd.5.1.7.fastq.gz</t>
+  </si>
+  <si>
+    <t>/local/path/to/rev.5.1.7.fastq.gz</t>
+  </si>
+  <si>
+    <t>CTTTPP518.00</t>
+  </si>
+  <si>
+    <t>/local/path/to/fwd.5.1.8.fastq.gz</t>
+  </si>
+  <si>
+    <t>/local/path/to/rev.5.1.8.fastq.gz</t>
   </si>
 </sst>
 </file>
@@ -544,7 +745,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
@@ -558,12 +759,13 @@
     <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1" indent="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1" indent="1"/>
-    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -905,7 +1107,7 @@
   <dimension ref="A1:G2012"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+      <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -917,10 +1119,10 @@
       <c r="A1" t="s">
         <v>68</v>
       </c>
-      <c r="B1" s="5" t="s">
+      <c r="B1" s="6" t="s">
         <v>69</v>
       </c>
-      <c r="C1" s="5"/>
+      <c r="C1" s="6"/>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
@@ -929,7 +1131,7 @@
       <c r="B2" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="6" t="s">
+      <c r="C2" s="5" t="s">
         <v>75</v>
       </c>
     </row>
@@ -940,7 +1142,7 @@
       <c r="B3" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="C3" s="6" t="s">
+      <c r="C3" s="5" t="s">
         <v>45</v>
       </c>
     </row>
@@ -951,7 +1153,7 @@
       <c r="B4" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="C4" s="6" t="s">
+      <c r="C4" s="5" t="s">
         <v>48</v>
       </c>
     </row>
@@ -962,7 +1164,7 @@
       <c r="B5" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="C5" s="6" t="s">
+      <c r="C5" s="5" t="s">
         <v>52</v>
       </c>
     </row>
@@ -973,7 +1175,7 @@
       <c r="B6" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="C6" s="6" t="s">
+      <c r="C6" s="5" t="s">
         <v>58</v>
       </c>
     </row>
@@ -984,7 +1186,7 @@
       <c r="B7" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="C7" s="6" t="s">
+      <c r="C7" s="5" t="s">
         <v>62</v>
       </c>
     </row>
@@ -995,7 +1197,7 @@
       <c r="B8" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="C8" s="6">
+      <c r="C8" s="5">
         <v>100</v>
       </c>
     </row>
@@ -1006,7 +1208,7 @@
       <c r="B9" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="C9" s="6" t="s">
+      <c r="C9" s="5" t="s">
         <v>64</v>
       </c>
     </row>
@@ -1014,14 +1216,14 @@
       <c r="A11" t="s">
         <v>71</v>
       </c>
-      <c r="B11" s="5" t="s">
+      <c r="B11" s="6" t="s">
         <v>72</v>
       </c>
-      <c r="C11" s="5"/>
-      <c r="D11" s="5"/>
-      <c r="E11" s="5"/>
-      <c r="F11" s="5"/>
-      <c r="G11" s="5"/>
+      <c r="C11" s="6"/>
+      <c r="D11" s="6"/>
+      <c r="E11" s="6"/>
+      <c r="F11" s="6"/>
+      <c r="G11" s="6"/>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
@@ -1050,178 +1252,592 @@
       <c r="A13" t="s">
         <v>74</v>
       </c>
+      <c r="B13" t="s">
+        <v>76</v>
+      </c>
+      <c r="C13">
+        <v>1</v>
+      </c>
+      <c r="D13" t="s">
+        <v>77</v>
+      </c>
+      <c r="E13" t="s">
+        <v>78</v>
+      </c>
+      <c r="F13" s="7">
+        <v>40179</v>
+      </c>
+      <c r="G13">
+        <v>1</v>
+      </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>74</v>
       </c>
+      <c r="B14" t="s">
+        <v>79</v>
+      </c>
+      <c r="C14">
+        <v>1</v>
+      </c>
+      <c r="D14" t="s">
+        <v>80</v>
+      </c>
+      <c r="E14" t="s">
+        <v>81</v>
+      </c>
+      <c r="F14" s="7">
+        <v>40179</v>
+      </c>
+      <c r="G14">
+        <v>1</v>
+      </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>74</v>
       </c>
+      <c r="B15" t="s">
+        <v>76</v>
+      </c>
+      <c r="C15">
+        <v>2</v>
+      </c>
+      <c r="D15" t="s">
+        <v>82</v>
+      </c>
+      <c r="E15" t="s">
+        <v>83</v>
+      </c>
+      <c r="F15" s="7">
+        <v>40179</v>
+      </c>
+      <c r="G15">
+        <v>1</v>
+      </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>74</v>
       </c>
-    </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B16" t="s">
+        <v>79</v>
+      </c>
+      <c r="C16">
+        <v>2</v>
+      </c>
+      <c r="D16" t="s">
+        <v>84</v>
+      </c>
+      <c r="E16" t="s">
+        <v>85</v>
+      </c>
+      <c r="F16" s="7">
+        <v>40179</v>
+      </c>
+      <c r="G16">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>74</v>
       </c>
-    </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B17" t="s">
+        <v>86</v>
+      </c>
+      <c r="C17">
+        <v>1</v>
+      </c>
+      <c r="D17" t="s">
+        <v>87</v>
+      </c>
+      <c r="E17" t="s">
+        <v>88</v>
+      </c>
+      <c r="F17" s="7">
+        <v>40179</v>
+      </c>
+      <c r="G17">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>74</v>
       </c>
-    </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B18" t="s">
+        <v>89</v>
+      </c>
+      <c r="C18">
+        <v>1</v>
+      </c>
+      <c r="D18" t="s">
+        <v>90</v>
+      </c>
+      <c r="E18" t="s">
+        <v>91</v>
+      </c>
+      <c r="F18" s="7">
+        <v>40179</v>
+      </c>
+      <c r="G18">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>74</v>
       </c>
-    </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B19" t="s">
+        <v>92</v>
+      </c>
+      <c r="C19">
+        <v>1</v>
+      </c>
+      <c r="D19" t="s">
+        <v>93</v>
+      </c>
+      <c r="E19" t="s">
+        <v>94</v>
+      </c>
+      <c r="F19" s="7">
+        <v>40179</v>
+      </c>
+      <c r="G19">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>74</v>
       </c>
-    </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B20" t="s">
+        <v>95</v>
+      </c>
+      <c r="C20">
+        <v>1</v>
+      </c>
+      <c r="D20" t="s">
+        <v>96</v>
+      </c>
+      <c r="E20" t="s">
+        <v>97</v>
+      </c>
+      <c r="F20" s="7">
+        <v>40179</v>
+      </c>
+      <c r="G20">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>74</v>
       </c>
-    </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B21" t="s">
+        <v>98</v>
+      </c>
+      <c r="C21">
+        <v>1</v>
+      </c>
+      <c r="D21" t="s">
+        <v>99</v>
+      </c>
+      <c r="E21" t="s">
+        <v>100</v>
+      </c>
+      <c r="F21" s="7">
+        <v>40179</v>
+      </c>
+      <c r="G21">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>74</v>
       </c>
-    </row>
-    <row r="23" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B22" t="s">
+        <v>101</v>
+      </c>
+      <c r="C22">
+        <v>1</v>
+      </c>
+      <c r="D22" t="s">
+        <v>102</v>
+      </c>
+      <c r="E22" t="s">
+        <v>103</v>
+      </c>
+      <c r="F22" s="7">
+        <v>40179</v>
+      </c>
+      <c r="G22">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>74</v>
       </c>
-    </row>
-    <row r="24" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B23" t="s">
+        <v>104</v>
+      </c>
+      <c r="C23">
+        <v>1</v>
+      </c>
+      <c r="D23" t="s">
+        <v>105</v>
+      </c>
+      <c r="E23" t="s">
+        <v>106</v>
+      </c>
+      <c r="F23" s="7">
+        <v>40179</v>
+      </c>
+      <c r="G23">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>74</v>
       </c>
-    </row>
-    <row r="25" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B24" t="s">
+        <v>107</v>
+      </c>
+      <c r="C24">
+        <v>1</v>
+      </c>
+      <c r="D24" t="s">
+        <v>108</v>
+      </c>
+      <c r="E24" t="s">
+        <v>109</v>
+      </c>
+      <c r="F24" s="7">
+        <v>40179</v>
+      </c>
+      <c r="G24">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>74</v>
       </c>
-    </row>
-    <row r="26" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B25" t="s">
+        <v>110</v>
+      </c>
+      <c r="C25">
+        <v>1</v>
+      </c>
+      <c r="D25" t="s">
+        <v>111</v>
+      </c>
+      <c r="E25" t="s">
+        <v>112</v>
+      </c>
+      <c r="F25" s="7">
+        <v>40179</v>
+      </c>
+      <c r="G25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>74</v>
       </c>
-    </row>
-    <row r="27" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B26" t="s">
+        <v>113</v>
+      </c>
+      <c r="C26">
+        <v>1</v>
+      </c>
+      <c r="D26" t="s">
+        <v>114</v>
+      </c>
+      <c r="E26" t="s">
+        <v>115</v>
+      </c>
+      <c r="F26" s="7">
+        <v>40179</v>
+      </c>
+      <c r="G26">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>74</v>
       </c>
-    </row>
-    <row r="28" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B27" t="s">
+        <v>116</v>
+      </c>
+      <c r="C27">
+        <v>1</v>
+      </c>
+      <c r="D27" t="s">
+        <v>117</v>
+      </c>
+      <c r="E27" t="s">
+        <v>118</v>
+      </c>
+      <c r="F27" s="7">
+        <v>40179</v>
+      </c>
+      <c r="G27">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>74</v>
       </c>
-    </row>
-    <row r="29" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B28" t="s">
+        <v>119</v>
+      </c>
+      <c r="C28">
+        <v>1</v>
+      </c>
+      <c r="D28" t="s">
+        <v>120</v>
+      </c>
+      <c r="E28" t="s">
+        <v>121</v>
+      </c>
+      <c r="F28" s="7">
+        <v>40179</v>
+      </c>
+      <c r="G28">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>74</v>
       </c>
-    </row>
-    <row r="30" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B29" t="s">
+        <v>122</v>
+      </c>
+      <c r="C29">
+        <v>1</v>
+      </c>
+      <c r="D29" t="s">
+        <v>123</v>
+      </c>
+      <c r="E29" t="s">
+        <v>124</v>
+      </c>
+      <c r="F29" s="7">
+        <v>40179</v>
+      </c>
+      <c r="G29">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>74</v>
       </c>
-    </row>
-    <row r="31" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B30" t="s">
+        <v>125</v>
+      </c>
+      <c r="C30">
+        <v>1</v>
+      </c>
+      <c r="D30" t="s">
+        <v>126</v>
+      </c>
+      <c r="E30" t="s">
+        <v>127</v>
+      </c>
+      <c r="F30" s="7">
+        <v>40179</v>
+      </c>
+      <c r="G30">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>74</v>
       </c>
-    </row>
-    <row r="32" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B31" t="s">
+        <v>128</v>
+      </c>
+      <c r="C31">
+        <v>1</v>
+      </c>
+      <c r="D31" t="s">
+        <v>129</v>
+      </c>
+      <c r="E31" t="s">
+        <v>130</v>
+      </c>
+      <c r="F31" s="7">
+        <v>40179</v>
+      </c>
+      <c r="G31">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>74</v>
       </c>
-    </row>
-    <row r="33" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B32" t="s">
+        <v>131</v>
+      </c>
+      <c r="C32">
+        <v>1</v>
+      </c>
+      <c r="D32" t="s">
+        <v>132</v>
+      </c>
+      <c r="E32" t="s">
+        <v>133</v>
+      </c>
+      <c r="F32" s="7">
+        <v>40179</v>
+      </c>
+      <c r="G32">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>74</v>
       </c>
-    </row>
-    <row r="34" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B33" t="s">
+        <v>134</v>
+      </c>
+      <c r="C33">
+        <v>1</v>
+      </c>
+      <c r="D33" t="s">
+        <v>135</v>
+      </c>
+      <c r="E33" t="s">
+        <v>136</v>
+      </c>
+      <c r="F33" s="7">
+        <v>40179</v>
+      </c>
+      <c r="G33">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>74</v>
       </c>
-    </row>
-    <row r="35" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B34" t="s">
+        <v>137</v>
+      </c>
+      <c r="C34">
+        <v>1</v>
+      </c>
+      <c r="D34" t="s">
+        <v>138</v>
+      </c>
+      <c r="E34" t="s">
+        <v>139</v>
+      </c>
+      <c r="F34" s="7">
+        <v>40179</v>
+      </c>
+      <c r="G34">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>74</v>
       </c>
-    </row>
-    <row r="36" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B35" t="s">
+        <v>140</v>
+      </c>
+      <c r="C35">
+        <v>1</v>
+      </c>
+      <c r="D35" t="s">
+        <v>141</v>
+      </c>
+      <c r="E35" t="s">
+        <v>142</v>
+      </c>
+      <c r="F35" s="7">
+        <v>40179</v>
+      </c>
+      <c r="G35">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="37" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="38" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="39" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="40" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="41" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="42" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="43" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="44" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="45" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="46" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="47" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="48" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>74</v>
       </c>
@@ -11052,8 +11668,8 @@
     <mergeCell ref="B11:G11"/>
   </mergeCells>
   <dataValidations count="6">
-    <dataValidation type="custom" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="Please enter date in format mm/dd/yyyy" sqref="F13:F2012" xr:uid="{00000000-0002-0000-0000-000006000000}">
-      <formula1>AND(ISNUMBER(F13:F2012),LEFT(CELL("format",F13:F2012),1)="D")</formula1>
+    <dataValidation type="custom" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="Please enter date in format mm/dd/yyyy" sqref="F36:F2012" xr:uid="{00000000-0002-0000-0000-000006000000}">
+      <formula1>AND(ISNUMBER(F36:F2035),LEFT(CELL("format",F36:F2035),1)="D")</formula1>
     </dataValidation>
     <dataValidation type="list" showInputMessage="1" showErrorMessage="1" sqref="C7" xr:uid="{88498756-4ABE-4DD3-A8D7-6554C538A6E2}">
       <formula1>"Paired,Single"</formula1>

</xml_diff>